<commit_message>
[IMP] New data for test environment
</commit_message>
<xml_diff>
--- a/z0bug_odoo/build/lib.linux-x86_64-2.7/z0bug_odoo/data/account_fiscal_position.xlsx
+++ b/z0bug_odoo/build/lib.linux-x86_64-2.7/z0bug_odoo/data/account_fiscal_position.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="85">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -28,6 +28,9 @@
     <t xml:space="preserve">_requirements</t>
   </si>
   <si>
+    <t xml:space="preserve">sequence</t>
+  </si>
+  <si>
     <t xml:space="preserve">name</t>
   </si>
   <si>
@@ -118,6 +121,30 @@
     <t xml:space="preserve">IVA al 4%</t>
   </si>
   <si>
+    <t xml:space="preserve">z0bug.fiscalpos_fr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EU-OSS FR – Francia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z0bug.fiscalpos_de</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EU-OSS DE – Germania</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z0bug.fiscalpos_es</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EU-OSS ES – Spagna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z0bug.fiscalpos_si</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EU-OSS SI – Slovenia</t>
+  </si>
+  <si>
     <t xml:space="preserve">z0bug.fiscalpos_at</t>
   </si>
   <si>
@@ -148,12 +175,6 @@
     <t xml:space="preserve">EU-OSS CZ – Rep. Ceca</t>
   </si>
   <si>
-    <t xml:space="preserve">z0bug.fiscalpos_de</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EU-OSS DE – Germania</t>
-  </si>
-  <si>
     <t xml:space="preserve">z0bug.fiscalpos_dk</t>
   </si>
   <si>
@@ -172,24 +193,12 @@
     <t xml:space="preserve">EU-OSS EL – Grecia</t>
   </si>
   <si>
-    <t xml:space="preserve">z0bug.fiscalpos_es</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EU-OSS ES – Spagna</t>
-  </si>
-  <si>
     <t xml:space="preserve">z0bug.fiscalpos_fi</t>
   </si>
   <si>
     <t xml:space="preserve">EU-OSS FI – Finlandia</t>
   </si>
   <si>
-    <t xml:space="preserve">z0bug.fiscalpos_fr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EU-OSS FR – Francia</t>
-  </si>
-  <si>
     <t xml:space="preserve">z0bug.fiscalpos_hr</t>
   </si>
   <si>
@@ -260,12 +269,6 @@
   </si>
   <si>
     <t xml:space="preserve">EU-OSS SE – Svezia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">z0bug.fiscalpos_si</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EU-OSS SI – Slovenia</t>
   </si>
   <si>
     <t xml:space="preserve">z0bug.fiscalpos_sk</t>
@@ -281,7 +284,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -302,11 +305,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -356,7 +354,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -377,22 +375,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K4" activeCellId="0" sqref="K4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="44.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="26.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="26.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -429,382 +428,484 @@
       <c r="K1" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="0" t="s">
         <v>12</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" s="0" t="s">
+      <c r="C3" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>15</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" s="0" t="s">
+      <c r="C4" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="0" t="s">
+      <c r="G4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="K4" s="0" t="s">
         <v>20</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="0" t="s">
-        <v>15</v>
+      <c r="C5" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="C6" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="C7" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="0" t="s">
         <v>31</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="C9" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="C10" s="0" t="n">
+        <v>101</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="F11" s="0" t="n">
+      <c r="C11" s="0" t="n">
+        <v>102</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="0" t="n">
+      <c r="C12" s="0" t="n">
+        <v>103</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="0" t="n">
+      <c r="C13" s="0" t="n">
+        <v>104</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="F14" s="0" t="n">
+      <c r="C14" s="0" t="n">
+        <v>105</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="G14" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="F15" s="0" t="n">
+      <c r="C15" s="0" t="n">
+        <v>106</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="F16" s="0" t="n">
+      <c r="C16" s="0" t="n">
+        <v>107</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="G16" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C17" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="F17" s="0" t="n">
+      <c r="C17" s="0" t="n">
+        <v>108</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="G17" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="C18" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="F18" s="0" t="n">
+      <c r="C18" s="0" t="n">
+        <v>109</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="G18" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="C19" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="F19" s="0" t="n">
+      <c r="C19" s="0" t="n">
+        <v>110</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="G19" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="C20" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="F20" s="0" t="n">
+      <c r="C20" s="0" t="n">
+        <v>111</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="G20" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="F21" s="0" t="n">
+      <c r="C21" s="0" t="n">
+        <v>112</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="G21" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="C22" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="F22" s="0" t="n">
+      <c r="C22" s="0" t="n">
+        <v>113</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="G22" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="C23" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="F23" s="0" t="n">
+      <c r="C23" s="0" t="n">
+        <v>114</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="G23" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="C24" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="F24" s="0" t="n">
+      <c r="C24" s="0" t="n">
+        <v>115</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="G24" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="C25" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="F25" s="0" t="n">
+      <c r="C25" s="0" t="n">
+        <v>116</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="G25" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="C26" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="F26" s="0" t="n">
+      <c r="C26" s="0" t="n">
+        <v>117</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="G26" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="C27" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="F27" s="0" t="n">
+      <c r="C27" s="0" t="n">
+        <v>118</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="G27" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="C28" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="F28" s="0" t="n">
+      <c r="C28" s="0" t="n">
+        <v>119</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="G28" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="C29" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="F29" s="0" t="n">
+      <c r="C29" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="G29" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="C30" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="F30" s="0" t="n">
+      <c r="C30" s="0" t="n">
+        <v>121</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="G30" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="C31" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="F31" s="0" t="n">
+      <c r="C31" s="0" t="n">
+        <v>122</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="G31" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="C32" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="F32" s="0" t="n">
+      <c r="C32" s="0" t="n">
+        <v>123</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="G32" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="C33" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="F33" s="0" t="n">
+      <c r="C33" s="0" t="n">
+        <v>124</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="G33" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="C34" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="F34" s="0" t="n">
+      <c r="C34" s="0" t="n">
+        <v>125</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="G34" s="0" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>